<commit_message>
Working parser (70%), next: block class.
</commit_message>
<xml_diff>
--- a/Track_Resources/Blue_Line_Block_Info.xlsx
+++ b/Track_Resources/Blue_Line_Block_Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhqu\OneDrive\Documents\GitHub\ECE-1140\Track_Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B1AF09-DB93-4E88-9D57-A6DED0221727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8C8FB0-FF69-4E98-97C8-C1E17695264C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23F08DD-D3F3-4876-AD25-C71E6A86591A}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,7 +536,7 @@
         <v>50</v>
       </c>
       <c r="E2" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="3">
         <v>50</v>
@@ -544,12 +544,11 @@
       <c r="G2" s="3"/>
       <c r="H2" s="1"/>
       <c r="I2" s="7">
-        <f>E2*D2/100</f>
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="J2" s="7">
         <f>I2</f>
-        <v>0</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
@@ -564,10 +563,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="3">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="3">
         <v>50</v>
@@ -575,17 +574,16 @@
       <c r="G3" s="3"/>
       <c r="H3" s="1"/>
       <c r="I3" s="7">
-        <f t="shared" ref="I3:I6" si="0">E3*D3/100</f>
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="J3" s="7">
         <f>I3+J2</f>
-        <v>0</v>
+        <v>4.3000000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="str">
-        <f t="shared" ref="A4:A16" si="1">A3</f>
+        <f t="shared" ref="A4:A16" si="0">A3</f>
         <v>Blue</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -595,10 +593,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="3">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4" s="3">
         <v>50</v>
@@ -608,17 +606,16 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="J4" s="7">
-        <f t="shared" ref="J4:J6" si="2">I4+J3</f>
-        <v>0</v>
+        <f t="shared" ref="J4:J6" si="1">I4+J3</f>
+        <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Blue</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -628,10 +625,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="3">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F5" s="3">
         <v>50</v>
@@ -639,17 +636,16 @@
       <c r="G5" s="3"/>
       <c r="H5" s="1"/>
       <c r="I5" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="J5" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Blue</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -659,10 +655,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="3">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E6" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F6" s="3">
         <v>50</v>
@@ -672,17 +668,16 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="J6" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>11.5</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Blue</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -692,10 +687,10 @@
         <v>6</v>
       </c>
       <c r="D7" s="3">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E7" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F7" s="3">
         <v>50</v>
@@ -705,17 +700,16 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="7">
-        <f t="shared" ref="I7:I16" si="3">E7*D7/100</f>
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="J7" s="7">
-        <f t="shared" ref="J7:J16" si="4">I7+J6</f>
-        <v>0</v>
+        <f t="shared" ref="J7:J16" si="2">I7+J6</f>
+        <v>14.1</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Blue</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -725,10 +719,10 @@
         <v>7</v>
       </c>
       <c r="D8" s="3">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E8" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F8" s="3">
         <v>50</v>
@@ -736,17 +730,16 @@
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="J8" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>16.8</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Blue</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -756,10 +749,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="3">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F9" s="3">
         <v>50</v>
@@ -767,17 +760,16 @@
       <c r="G9" s="3"/>
       <c r="H9" s="1"/>
       <c r="I9" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="J9" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Blue</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -787,10 +779,10 @@
         <v>9</v>
       </c>
       <c r="D10" s="3">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E10" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F10" s="3">
         <v>50</v>
@@ -800,17 +792,16 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="J10" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>22.5</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Blue</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -820,10 +811,10 @@
         <v>10</v>
       </c>
       <c r="D11" s="3">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E11" s="3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3">
         <v>50</v>
@@ -833,17 +824,16 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>25.5</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Blue</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -853,10 +843,10 @@
         <v>11</v>
       </c>
       <c r="D12" s="3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E12" s="3">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F12" s="3">
         <v>50</v>
@@ -866,17 +856,16 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="J12" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>28.6</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Blue</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -886,10 +875,10 @@
         <v>12</v>
       </c>
       <c r="D13" s="3">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E13" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F13" s="3">
         <v>50</v>
@@ -897,17 +886,16 @@
       <c r="G13" s="3"/>
       <c r="H13" s="1"/>
       <c r="I13" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="J13" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>31.8</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Blue</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -917,10 +905,10 @@
         <v>13</v>
       </c>
       <c r="D14" s="3">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E14" s="3">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F14" s="3">
         <v>50</v>
@@ -928,17 +916,16 @@
       <c r="G14" s="3"/>
       <c r="H14" s="1"/>
       <c r="I14" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="J14" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>35.1</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Blue</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -948,10 +935,10 @@
         <v>14</v>
       </c>
       <c r="D15" s="3">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E15" s="3">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F15" s="3">
         <v>50</v>
@@ -961,17 +948,16 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.4</v>
       </c>
       <c r="J15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>38.5</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Blue</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -981,10 +967,10 @@
         <v>15</v>
       </c>
       <c r="D16" s="3">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E16" s="3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F16" s="3">
         <v>50</v>
@@ -994,12 +980,11 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="J16" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Iteration 2 done for now!
</commit_message>
<xml_diff>
--- a/Track_Resources/Blue_Line_Block_Info.xlsx
+++ b/Track_Resources/Blue_Line_Block_Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhqu\OneDrive\Documents\GitHub\ECE-1140\Track_Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8C8FB0-FF69-4E98-97C8-C1E17695264C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72616A2B-CFFB-4274-9D32-03D952BB7D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,7 +482,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1002,5 +1002,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>